<commit_message>
20201130 CRE20-015-02	Special Support Scheme for Continuing Medical Care to HA Patients in GD (SSSCMC) – Phase 2 (Reimbursement)
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSM0013-PreAuthorizationSSSCMC_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSM0013-PreAuthorizationSSSCMC_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\EHS2019_BatchUpload\ExcelGenerator\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-0XX (HA Scheme)\Front-end (Phase 2 - Reimburse)\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,12 +20,12 @@
     <sheet name="备注" sheetId="4" r:id="rId6"/>
     <sheet name="变更记录" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -488,15 +488,11 @@
     <t>用户资料 (姓名/身份证号码)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
-  <si>
-    <t>二级科室</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="d\ mmm\ yyyy\ h:mm"/>
     <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
@@ -1713,7 +1709,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1722,28 +1718,27 @@
     <col min="1" max="1" width="8.625" style="46" customWidth="1"/>
     <col min="2" max="2" width="18.125" style="5" customWidth="1"/>
     <col min="3" max="3" width="25.125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="18.625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="21.375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="22.625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="73" customWidth="1"/>
-    <col min="8" max="9" width="13.375" style="73" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.875" style="50" customWidth="1"/>
-    <col min="11" max="11" width="23.5" style="50" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.75" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="10"/>
+    <col min="4" max="4" width="21.375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.625" style="49" customWidth="1"/>
+    <col min="6" max="6" width="13.375" style="73" customWidth="1"/>
+    <col min="7" max="8" width="13.375" style="73" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.875" style="50" customWidth="1"/>
+    <col min="10" max="10" width="23.5" style="50" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.75" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16.5">
+    <row r="1" spans="1:14" ht="16.5">
       <c r="A1" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="53"/>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="J1" s="53"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="5"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:15" s="14" customFormat="1" ht="70.5" customHeight="1">
+      <c r="J2" s="53"/>
+    </row>
+    <row r="3" spans="1:14" s="14" customFormat="1" ht="70.5" customHeight="1">
       <c r="A3" s="79" t="s">
         <v>32</v>
       </c>
@@ -1753,50 +1748,46 @@
       <c r="C3" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="80" t="s">
-        <v>71</v>
+      <c r="D3" s="48" t="s">
+        <v>2</v>
       </c>
       <c r="E3" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="48" t="s">
         <v>4</v>
       </c>
+      <c r="F3" s="74" t="s">
+        <v>64</v>
+      </c>
       <c r="G3" s="74" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H3" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="I3" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="J3" s="48" t="s">
         <v>6</v>
       </c>
+      <c r="L3" s="12"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-    </row>
-    <row r="4" spans="1:15" s="5" customFormat="1">
+    </row>
+    <row r="4" spans="1:14" s="5" customFormat="1">
       <c r="A4" s="2"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="72"/>
       <c r="G4" s="72"/>
       <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
+      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>